<commit_message>
New version of regioinvent + moved to EI3.10
</commit_message>
<xml_diff>
--- a/data/Mining_production_data/canada_site_specific_production_data.xlsx
+++ b/data/Mining_production_data/canada_site_specific_production_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/marin_pellan_polymtlus_ca/Documents/Desktop/POST_DOC/Project/regionalized_lci_mineral/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/marin_pellan_polymtlus_ca/Documents/Desktop/POST_DOC/Project/regionalized_lci_mineral/data/Mining_production_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="11_F25DC773A252ABDACC104887411C794C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A88560FF-ABF6-4820-AAC2-2FAEBBDF6A75}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="11_F25DC773A252ABDACC104887411C794C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C560EC5A-EB92-4757-905D-DE1B65EF0936}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9149" uniqueCount="3756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9156" uniqueCount="3763">
   <si>
     <t>company1</t>
   </si>
@@ -11395,9 +11395,6 @@
     <t>Nickel-copper sulfide ore bodies, which also contain cobalt.</t>
   </si>
   <si>
-    <t>Processing plant: Nickel concentrate from Voisey’s Bay (Labrador) is refined at Long Harbour (Newfoundland) to produce finished nickel rounds, as well as associated copper and cobalt products. Since the second half of 2021, Long Harbour also started processing additional feed from Thompson, Manitoba. Copper concentrate produced by Voisey’s Bay (Labrador) is directly sold to the market. Other facilities: Waste and tailings disposal structures. Logistics: The copper and nickel concentrate from Voisey’s Bay are transported to the port by haulage trucks and then shipped by dry bulk vessels to either overseas markets (copper) or to our Long Harbour facilities (nickel) for further processing. Thompson concentrate is sent to Long Harbour by rail and ship. Energy: Power at Voisey’s Bay is 100% supplied through Vale-owned diesel generators. Power at the Long Harbour refinery is supplied by the Newfoundland and Labrador provincial utility company.</t>
-  </si>
-  <si>
     <t>50,000 t of nickel metal in concentrate
 32,000 t of copper metal in concentrate</t>
   </si>
@@ -11438,6 +11435,30 @@
   </si>
   <si>
     <t>https://www.glencore.ca/en/sudburyino/</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Source file from Dallaire-Fortier's article</t>
+  </si>
+  <si>
+    <t>Data includes company and facility name, city and province, coordinates, list of commodities, mining type, ore type, production volume for the latest year available and a brief description. Links to relevant sources of information (e.g. MinDat, MDA and company reports) are also provided</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Production_reference_year</t>
+  </si>
+  <si>
+    <t>2015 (from MDA)</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No production data from company report, only reserves data </t>
   </si>
 </sst>
 </file>
@@ -11525,7 +11546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -11535,23 +11556,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11569,10 +11599,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11841,16 +11867,16 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -11888,8 +11914,22 @@
       <c r="A8" t="s">
         <v>3686</v>
       </c>
+      <c r="B8" t="s">
+        <v>3756</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>3687</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3757</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3758</v>
       </c>
     </row>
   </sheetData>
@@ -11902,10 +11942,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B83351-2AED-4DFF-AD62-073740819681}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11919,12 +11959,17 @@
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="19.21875" customWidth="1"/>
-    <col min="11" max="11" width="33.77734375" customWidth="1"/>
-    <col min="12" max="12" width="48.77734375" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.77734375" customWidth="1"/>
+    <col min="13" max="14" width="48.77734375" customWidth="1"/>
+    <col min="15" max="15" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="116.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>3728</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -11945,7 +11990,7 @@
       <c r="G1" s="4" t="s">
         <v>3692</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>3729</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -11955,499 +12000,529 @@
         <v>3742</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>3759</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>3730</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>3736</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>3761</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>3731</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>3732</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>3738</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>3693</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>3694</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>3695</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="8">
         <v>56.337780000000002</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="8">
         <v>-62.0944</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="9" t="s">
         <v>1933</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="10" t="s">
         <v>3741</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="9" t="s">
         <v>3743</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="9" t="s">
+        <v>3760</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>3744</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>3737</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>3762</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>3735</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>3733</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>3739</v>
+      </c>
+      <c r="R2" s="9"/>
+    </row>
+    <row r="3" spans="1:18" s="7" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>3696</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3697</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="8">
+        <v>61.691600000000001</v>
+      </c>
+      <c r="G3" s="8">
+        <v>-73.666600000000003</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1513</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>3749</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>3751</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>3747</v>
+      </c>
+      <c r="N3" s="9"/>
+      <c r="O3" s="7" t="s">
+        <v>3746</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>3745</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>3737</v>
-      </c>
-      <c r="M2" t="s">
-        <v>3735</v>
-      </c>
-      <c r="N2" t="s">
-        <v>3733</v>
-      </c>
-      <c r="O2" t="s">
-        <v>3739</v>
-      </c>
-      <c r="P2" t="s">
-        <v>3744</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="Q3" s="7" t="s">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="7" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>1504</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>3696</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3697</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="5">
-        <v>61.691600000000001</v>
-      </c>
-      <c r="G3" s="5">
-        <v>-73.666600000000003</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>1513</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="B4" s="8" t="s">
+        <v>3698</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>3699</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>3700</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="8">
+        <v>46.674199999999999</v>
+      </c>
+      <c r="G4" s="8">
+        <v>-81.342500000000001</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="L4" s="7" t="s">
+        <v>3751</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>3750</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N4" s="9"/>
+      <c r="O4" s="7" t="s">
+        <v>3753</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>3752</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>3748</v>
-      </c>
-      <c r="M3" t="s">
-        <v>3747</v>
-      </c>
-      <c r="N3" t="s">
-        <v>3746</v>
-      </c>
-      <c r="O3" t="s">
-        <v>3749</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="Q4" s="7" t="s">
+        <v>3754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="8" t="s">
+        <v>3494</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>3701</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>1997</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
+        <v>46.494999999999997</v>
+      </c>
+      <c r="G5" s="8">
+        <v>-81.056100000000001</v>
+      </c>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>3702</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
+        <v>55.712859999999999</v>
+      </c>
+      <c r="G6" s="8">
+        <v>-97.851060000000004</v>
+      </c>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>3698</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>3699</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>3700</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="5">
-        <v>46.674199999999999</v>
-      </c>
-      <c r="G4" s="5">
-        <v>-81.342500000000001</v>
-      </c>
-      <c r="K4" t="s">
-        <v>3752</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>3751</v>
-      </c>
-      <c r="M4" t="s">
-        <v>3754</v>
-      </c>
-      <c r="N4" t="s">
-        <v>3753</v>
-      </c>
-      <c r="O4" t="s">
-        <v>3755</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C7" s="8" t="s">
+        <v>3704</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>3705</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8">
+        <v>46.658000000000001</v>
+      </c>
+      <c r="G7" s="8">
+        <v>-80.797200000000004</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B8" s="8" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>3706</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>1570</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8">
+        <v>46.638629999999999</v>
+      </c>
+      <c r="G8" s="8">
+        <v>-81.399760000000001</v>
+      </c>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>3494</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>3701</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C9" s="8" t="s">
+        <v>3707</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>3708</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
+        <v>46.566699999999997</v>
+      </c>
+      <c r="G9" s="8">
+        <v>-80.856200000000001</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="8" t="s">
+        <v>3709</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>3710</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8">
+        <v>46.381300000000003</v>
+      </c>
+      <c r="G10" s="8">
+        <v>-81.454099999999997</v>
+      </c>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="8" t="s">
+        <v>3711</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>1997</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
-        <v>46.494999999999997</v>
-      </c>
-      <c r="G5" s="5">
-        <v>-81.056100000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8">
+        <v>46.474600000000002</v>
+      </c>
+      <c r="G11" s="8">
+        <v>-81.090999999999994</v>
+      </c>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>3702</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>3703</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>1993</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5">
-        <v>55.712859999999999</v>
-      </c>
-      <c r="G6" s="5">
-        <v>-97.851060000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B12" s="8" t="s">
+        <v>3712</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>3713</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>3714</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8">
+        <v>61.563858000000003</v>
+      </c>
+      <c r="G12" s="8">
+        <v>-73.437360999999996</v>
+      </c>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>3698</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>3704</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>3705</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5">
-        <v>46.658000000000001</v>
-      </c>
-      <c r="G7" s="5">
-        <v>-80.797200000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B13" s="12" t="s">
+        <v>3494</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>3715</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>3716</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8">
+        <v>46.472900000000003</v>
+      </c>
+      <c r="G13" s="8">
+        <v>-81.185400000000001</v>
+      </c>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="8" t="s">
+        <v>3717</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>3718</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8">
+        <v>46.431249999999999</v>
+      </c>
+      <c r="G14" s="8">
+        <v>-81.349609999999998</v>
+      </c>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>2173</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>3719</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>3720</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8">
+        <v>48.361199999999997</v>
+      </c>
+      <c r="G15" s="8">
+        <v>-81.116600000000005</v>
+      </c>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>3494</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>3721</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>1570</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8">
+        <v>46.643500000000003</v>
+      </c>
+      <c r="G16" s="8">
+        <v>-81.383600000000001</v>
+      </c>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="8" t="s">
+        <v>3722</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8">
+        <v>46.532699999999998</v>
+      </c>
+      <c r="G17" s="8">
+        <v>-80.997600000000006</v>
+      </c>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="8" t="s">
+        <v>3723</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>1997</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8">
+        <v>46.459000000000003</v>
+      </c>
+      <c r="G18" s="8">
+        <v>-81.075800000000001</v>
+      </c>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>1565</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>3706</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C19" s="8" t="s">
+        <v>3724</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>1570</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5">
-        <v>46.638629999999999</v>
-      </c>
-      <c r="G8" s="5">
-        <v>-81.399760000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="E19" s="8"/>
+      <c r="F19" s="8">
+        <v>46.6599</v>
+      </c>
+      <c r="G19" s="8">
+        <v>-81.376499999999993</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>3494</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>3707</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>3708</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5">
-        <v>46.566699999999997</v>
-      </c>
-      <c r="G9" s="5">
-        <v>-80.856200000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C20" s="8" t="s">
+        <v>3725</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>3716</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8">
+        <v>46.457999999999998</v>
+      </c>
+      <c r="G20" s="8">
+        <v>-81.211500000000001</v>
+      </c>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="5" t="s">
-        <v>3709</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>3710</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5">
-        <v>46.381300000000003</v>
-      </c>
-      <c r="G10" s="5">
-        <v>-81.454099999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>956</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="5" t="s">
-        <v>3711</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>1997</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5">
-        <v>46.474600000000002</v>
-      </c>
-      <c r="G11" s="5">
-        <v>-81.090999999999994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>956</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>3712</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>3713</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>3714</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5">
-        <v>61.563858000000003</v>
-      </c>
-      <c r="G12" s="5">
-        <v>-73.437360999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>956</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>3494</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>3715</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>3716</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5">
-        <v>46.472900000000003</v>
-      </c>
-      <c r="G13" s="5">
-        <v>-81.185400000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>956</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="5" t="s">
-        <v>3717</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>3718</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5">
-        <v>46.431249999999999</v>
-      </c>
-      <c r="G14" s="5">
-        <v>-81.349609999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>956</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>2173</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>3719</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>3720</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5">
-        <v>48.361199999999997</v>
-      </c>
-      <c r="G15" s="5">
-        <v>-81.116600000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>956</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>3494</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>3721</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>1570</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5">
-        <v>46.643500000000003</v>
-      </c>
-      <c r="G16" s="5">
-        <v>-81.383600000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>956</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="5" t="s">
-        <v>3722</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>1429</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5">
-        <v>46.532699999999998</v>
-      </c>
-      <c r="G17" s="5">
-        <v>-80.997600000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>956</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="5" t="s">
-        <v>3723</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>1997</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5">
-        <v>46.459000000000003</v>
-      </c>
-      <c r="G18" s="5">
-        <v>-81.075800000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>956</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>1565</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>3724</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>1570</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5">
-        <v>46.6599</v>
-      </c>
-      <c r="G19" s="5">
-        <v>-81.376499999999993</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>956</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>3494</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>3725</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>3716</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5">
-        <v>46.457999999999998</v>
-      </c>
-      <c r="G20" s="5">
-        <v>-81.211500000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>956</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>1565</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="8" t="s">
         <v>3726</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="8" t="s">
         <v>3727</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8">
         <v>46.413060000000002</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="8">
         <v>-81.384240000000005</v>
       </c>
+      <c r="H21" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -12455,6 +12530,11 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B16:B18"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{C53822E9-C2A3-4D80-9744-885170CF2672}"/>
+    <hyperlink ref="Q2" r:id="rId2" xr:uid="{04E9B177-C74F-4B75-9D42-33FEBA8A9957}"/>
+    <hyperlink ref="P2" r:id="rId3" xr:uid="{809C1379-83BB-4058-9138-1479AA9A0C68}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12464,8 +12544,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AJ948"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A812" workbookViewId="0">
-      <selection activeCell="AH1" sqref="A1:AH932"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="F864" sqref="F864"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>